<commit_message>
small fixes for task-3
</commit_message>
<xml_diff>
--- a/Lab2/Task-3/Data.xlsx
+++ b/Lab2/Task-3/Data.xlsx
@@ -359,707 +359,707 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="n">
-        <v>13.0184577572279</v>
+        <v>25.92718227809252</v>
       </c>
       <c r="B1" t="n">
-        <v>10.57560473868229</v>
+        <v>13.65578108662694</v>
       </c>
       <c r="C1" t="n">
-        <v>1.853464245101432</v>
+        <v>27.71006605668829</v>
       </c>
       <c r="D1" t="n">
-        <v>27.84398267058961</v>
+        <v>7.910039432272094</v>
       </c>
       <c r="E1" t="n">
-        <v>17.95494076259767</v>
+        <v>26.7473686363864</v>
       </c>
       <c r="F1" t="n">
-        <v>6.992335178103898</v>
+        <v>25.94674647443332</v>
       </c>
       <c r="G1" t="n">
-        <v>7.45508702561169</v>
+        <v>21.02766578514784</v>
       </c>
       <c r="H1" t="n">
-        <v>13.74536923528972</v>
+        <v>9.006345202225754</v>
       </c>
       <c r="I1" t="n">
-        <v>3.982111724255501</v>
+        <v>10.30789802559425</v>
       </c>
       <c r="J1" t="n">
-        <v>7.004776158445634</v>
+        <v>26.4828424409353</v>
       </c>
       <c r="K1" t="n">
-        <v>25.11228262582343</v>
+        <v>3.071574792433862</v>
       </c>
       <c r="L1" t="n">
-        <v>15.30916041125678</v>
+        <v>8.735876604905631</v>
       </c>
       <c r="M1" t="n">
-        <v>21.93549423252064</v>
+        <v>29.533812194501</v>
       </c>
       <c r="N1" t="n">
-        <v>11.45105133842124</v>
+        <v>1.727206190720807</v>
       </c>
       <c r="O1" t="n">
-        <v>27.29826827595777</v>
+        <v>2.32165797744991</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="n">
-        <v>12.38538841340921</v>
+        <v>20.15770125058977</v>
       </c>
       <c r="B2" t="n">
-        <v>29.96258999283963</v>
+        <v>1.450994709476593</v>
       </c>
       <c r="C2" t="n">
-        <v>7.784599124610965</v>
+        <v>8.784064384793648</v>
       </c>
       <c r="D2" t="n">
-        <v>19.98850429008359</v>
+        <v>11.3309660173357</v>
       </c>
       <c r="E2" t="n">
-        <v>19.09192516680929</v>
+        <v>26.04615144564942</v>
       </c>
       <c r="F2" t="n">
-        <v>5.30938189512899</v>
+        <v>27.62830356771391</v>
       </c>
       <c r="G2" t="n">
-        <v>7.751817107284073</v>
+        <v>19.79424949414</v>
       </c>
       <c r="H2" t="n">
-        <v>28.73240645316914</v>
+        <v>29.20483818295027</v>
       </c>
       <c r="I2" t="n">
-        <v>17.65115430236724</v>
+        <v>4.913380421086946</v>
       </c>
       <c r="J2" t="n">
-        <v>10.46182766763959</v>
+        <v>26.28852095168888</v>
       </c>
       <c r="K2" t="n">
-        <v>7.766317005976656</v>
+        <v>17.26487618154057</v>
       </c>
       <c r="L2" t="n">
-        <v>9.006813207513972</v>
+        <v>1.218753656114688</v>
       </c>
       <c r="M2" t="n">
-        <v>25.26826521124037</v>
+        <v>18.22760923647114</v>
       </c>
       <c r="N2" t="n">
-        <v>3.207824944437538</v>
+        <v>24.8416834608759</v>
       </c>
       <c r="O2" t="n">
-        <v>17.70896113805315</v>
+        <v>6.734479217225015</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="n">
-        <v>7.980810953617325</v>
+        <v>20.86540690842241</v>
       </c>
       <c r="B3" t="n">
-        <v>27.24979948123124</v>
+        <v>3.450433580973494</v>
       </c>
       <c r="C3" t="n">
-        <v>27.33990207351491</v>
+        <v>7.355774208074092</v>
       </c>
       <c r="D3" t="n">
-        <v>15.39375703239375</v>
+        <v>27.27335670502888</v>
       </c>
       <c r="E3" t="n">
-        <v>14.03700331759223</v>
+        <v>18.23571952212412</v>
       </c>
       <c r="F3" t="n">
-        <v>8.377304768027425</v>
+        <v>19.60901616593736</v>
       </c>
       <c r="G3" t="n">
-        <v>19.09339711885752</v>
+        <v>28.94050355056864</v>
       </c>
       <c r="H3" t="n">
-        <v>7.787326125474785</v>
+        <v>18.67931166116659</v>
       </c>
       <c r="I3" t="n">
-        <v>8.26703382031746</v>
+        <v>2.481793334315846</v>
       </c>
       <c r="J3" t="n">
-        <v>26.97945796126952</v>
+        <v>23.08853847460831</v>
       </c>
       <c r="K3" t="n">
-        <v>26.8585147931615</v>
+        <v>11.13888500375606</v>
       </c>
       <c r="L3" t="n">
-        <v>24.18805764324017</v>
+        <v>26.44479386430688</v>
       </c>
       <c r="M3" t="n">
-        <v>24.09915409065747</v>
+        <v>26.51360782181713</v>
       </c>
       <c r="N3" t="n">
-        <v>13.57401342984904</v>
+        <v>22.03459177630727</v>
       </c>
       <c r="O3" t="n">
-        <v>12.51687192337878</v>
+        <v>20.99471556347149</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="n">
-        <v>1.953252663663197</v>
+        <v>7.373482331144545</v>
       </c>
       <c r="B4" t="n">
-        <v>27.28600373566898</v>
+        <v>20.66575447224554</v>
       </c>
       <c r="C4" t="n">
-        <v>18.04876485056905</v>
+        <v>11.29363265627161</v>
       </c>
       <c r="D4" t="n">
-        <v>29.79152410908658</v>
+        <v>22.21255412074022</v>
       </c>
       <c r="E4" t="n">
-        <v>19.59428189546548</v>
+        <v>26.76403648387036</v>
       </c>
       <c r="F4" t="n">
-        <v>21.19961102426824</v>
+        <v>13.46733099186202</v>
       </c>
       <c r="G4" t="n">
-        <v>4.623132560043616</v>
+        <v>29.8646498160022</v>
       </c>
       <c r="H4" t="n">
-        <v>27.42728018221711</v>
+        <v>26.65857581369774</v>
       </c>
       <c r="I4" t="n">
-        <v>5.761379655200847</v>
+        <v>8.138160518515273</v>
       </c>
       <c r="J4" t="n">
-        <v>28.78779086175043</v>
+        <v>24.54383608154318</v>
       </c>
       <c r="K4" t="n">
-        <v>5.070432352539203</v>
+        <v>1.616779998722623</v>
       </c>
       <c r="L4" t="n">
-        <v>5.205739284906482</v>
+        <v>25.57788298418383</v>
       </c>
       <c r="M4" t="n">
-        <v>3.689798541202989</v>
+        <v>29.84387676462801</v>
       </c>
       <c r="N4" t="n">
-        <v>19.59084404656489</v>
+        <v>21.24367316605093</v>
       </c>
       <c r="O4" t="n">
-        <v>18.38647460710736</v>
+        <v>6.358287878375246</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="n">
-        <v>28.02329231882102</v>
+        <v>14.4889673995826</v>
       </c>
       <c r="B5" t="n">
-        <v>13.08712650795794</v>
+        <v>20.44250054911469</v>
       </c>
       <c r="C5" t="n">
-        <v>19.08671659357019</v>
+        <v>4.191709995990229</v>
       </c>
       <c r="D5" t="n">
-        <v>17.38927023840412</v>
+        <v>11.9164784218025</v>
       </c>
       <c r="E5" t="n">
-        <v>13.84894384409763</v>
+        <v>4.459209369497922</v>
       </c>
       <c r="F5" t="n">
-        <v>9.988807078267889</v>
+        <v>14.24681002363393</v>
       </c>
       <c r="G5" t="n">
-        <v>7.755748992173585</v>
+        <v>12.42363938345982</v>
       </c>
       <c r="H5" t="n">
-        <v>23.85025186258967</v>
+        <v>2.737444558477874</v>
       </c>
       <c r="I5" t="n">
-        <v>18.69007602220815</v>
+        <v>29.35838722390753</v>
       </c>
       <c r="J5" t="n">
-        <v>11.59176968029276</v>
+        <v>5.19944245095222</v>
       </c>
       <c r="K5" t="n">
-        <v>21.44350255354169</v>
+        <v>28.66840657661794</v>
       </c>
       <c r="L5" t="n">
-        <v>18.00270497630635</v>
+        <v>29.52545579582688</v>
       </c>
       <c r="M5" t="n">
-        <v>7.656012438204246</v>
+        <v>22.41394137553782</v>
       </c>
       <c r="N5" t="n">
-        <v>15.77235798576829</v>
+        <v>12.88352701473961</v>
       </c>
       <c r="O5" t="n">
-        <v>16.8535349058656</v>
+        <v>14.89212698844447</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="n">
-        <v>7.275218507380306</v>
+        <v>12.58851111904495</v>
       </c>
       <c r="B6" t="n">
-        <v>18.41611675777074</v>
+        <v>17.25593964634868</v>
       </c>
       <c r="C6" t="n">
-        <v>8.398580508141405</v>
+        <v>27.08093052878391</v>
       </c>
       <c r="D6" t="n">
-        <v>24.69748109271305</v>
+        <v>17.10026196179122</v>
       </c>
       <c r="E6" t="n">
-        <v>8.373038535195384</v>
+        <v>10.49755827512746</v>
       </c>
       <c r="F6" t="n">
-        <v>7.392041093397737</v>
+        <v>2.051523546837716</v>
       </c>
       <c r="G6" t="n">
-        <v>2.928271976045129</v>
+        <v>24.17875529724298</v>
       </c>
       <c r="H6" t="n">
-        <v>27.88312593298648</v>
+        <v>22.10064362575594</v>
       </c>
       <c r="I6" t="n">
-        <v>19.37778622377092</v>
+        <v>3.590911208515566</v>
       </c>
       <c r="J6" t="n">
-        <v>28.57690918898955</v>
+        <v>26.44669027346433</v>
       </c>
       <c r="K6" t="n">
-        <v>9.511672192907495</v>
+        <v>21.60741330156816</v>
       </c>
       <c r="L6" t="n">
-        <v>19.52605590578519</v>
+        <v>22.41943350393503</v>
       </c>
       <c r="M6" t="n">
-        <v>28.0096258142774</v>
+        <v>16.60143450419001</v>
       </c>
       <c r="N6" t="n">
-        <v>5.454561354512408</v>
+        <v>5.665820019811048</v>
       </c>
       <c r="O6" t="n">
-        <v>21.69052683962044</v>
+        <v>25.2866829055219</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="n">
-        <v>23.9717835170011</v>
+        <v>12.08259603383189</v>
       </c>
       <c r="B7" t="n">
-        <v>27.40730088336908</v>
+        <v>15.23282665543521</v>
       </c>
       <c r="C7" t="n">
-        <v>19.26723413535166</v>
+        <v>8.429325914113431</v>
       </c>
       <c r="D7" t="n">
-        <v>24.44960629014875</v>
+        <v>11.54686572319147</v>
       </c>
       <c r="E7" t="n">
-        <v>15.14766154761512</v>
+        <v>16.82423756822132</v>
       </c>
       <c r="F7" t="n">
-        <v>14.62667357720268</v>
+        <v>16.66775687050954</v>
       </c>
       <c r="G7" t="n">
-        <v>22.17151425339354</v>
+        <v>10.54164788901882</v>
       </c>
       <c r="H7" t="n">
-        <v>29.04716705403951</v>
+        <v>5.937007833692081</v>
       </c>
       <c r="I7" t="n">
-        <v>13.76685989575028</v>
+        <v>9.850296071111124</v>
       </c>
       <c r="J7" t="n">
-        <v>12.0081010070843</v>
+        <v>12.32406277207107</v>
       </c>
       <c r="K7" t="n">
-        <v>7.226032407042323</v>
+        <v>6.495115581432477</v>
       </c>
       <c r="L7" t="n">
-        <v>4.668678240349259</v>
+        <v>13.16966543319803</v>
       </c>
       <c r="M7" t="n">
-        <v>2.061646016703783</v>
+        <v>11.16623041499016</v>
       </c>
       <c r="N7" t="n">
-        <v>26.11988608667926</v>
+        <v>19.33771617287197</v>
       </c>
       <c r="O7" t="n">
-        <v>17.19993451780205</v>
+        <v>3.703895796245941</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="n">
-        <v>16.52558417489424</v>
+        <v>15.243974615202</v>
       </c>
       <c r="B8" t="n">
-        <v>18.11285092740572</v>
+        <v>28.15791846773456</v>
       </c>
       <c r="C8" t="n">
-        <v>1.391444539633281</v>
+        <v>21.28625891985301</v>
       </c>
       <c r="D8" t="n">
-        <v>19.44364759871536</v>
+        <v>12.90898736051674</v>
       </c>
       <c r="E8" t="n">
-        <v>20.22225871780254</v>
+        <v>3.558429584525522</v>
       </c>
       <c r="F8" t="n">
-        <v>25.2214345581754</v>
+        <v>1.222139359567321</v>
       </c>
       <c r="G8" t="n">
-        <v>4.117984094673087</v>
+        <v>10.29681449979964</v>
       </c>
       <c r="H8" t="n">
-        <v>6.6391580799003</v>
+        <v>24.48553650820482</v>
       </c>
       <c r="I8" t="n">
-        <v>15.71990858423947</v>
+        <v>11.6492200706358</v>
       </c>
       <c r="J8" t="n">
-        <v>19.86103372156688</v>
+        <v>27.80417192144546</v>
       </c>
       <c r="K8" t="n">
-        <v>10.8697805054265</v>
+        <v>20.04650391289548</v>
       </c>
       <c r="L8" t="n">
-        <v>17.27898058994445</v>
+        <v>4.410772514586058</v>
       </c>
       <c r="M8" t="n">
-        <v>7.814510761098164</v>
+        <v>25.30041141519226</v>
       </c>
       <c r="N8" t="n">
-        <v>9.367181575629884</v>
+        <v>9.262166491454508</v>
       </c>
       <c r="O8" t="n">
-        <v>6.666120091362632</v>
+        <v>1.489841307158386</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="n">
-        <v>14.87798355147012</v>
+        <v>3.867765299773526</v>
       </c>
       <c r="B9" t="n">
-        <v>4.866676558782856</v>
+        <v>4.957555062332055</v>
       </c>
       <c r="C9" t="n">
-        <v>25.79169053027861</v>
+        <v>8.180042760935141</v>
       </c>
       <c r="D9" t="n">
-        <v>14.27417687989426</v>
+        <v>22.73067325031145</v>
       </c>
       <c r="E9" t="n">
-        <v>29.95201937000902</v>
+        <v>26.26517405928889</v>
       </c>
       <c r="F9" t="n">
-        <v>7.938596266332668</v>
+        <v>2.096569759411483</v>
       </c>
       <c r="G9" t="n">
-        <v>24.7746800917751</v>
+        <v>5.63012458336043</v>
       </c>
       <c r="H9" t="n">
-        <v>10.35516378991814</v>
+        <v>10.65610111097597</v>
       </c>
       <c r="I9" t="n">
-        <v>24.88036903722805</v>
+        <v>9.023389875049221</v>
       </c>
       <c r="J9" t="n">
-        <v>27.55003980062248</v>
+        <v>20.0727060877417</v>
       </c>
       <c r="K9" t="n">
-        <v>17.17366737980904</v>
+        <v>26.68963346623893</v>
       </c>
       <c r="L9" t="n">
-        <v>29.7710749099352</v>
+        <v>16.19644497369756</v>
       </c>
       <c r="M9" t="n">
-        <v>28.92042148854428</v>
+        <v>6.284949053738711</v>
       </c>
       <c r="N9" t="n">
-        <v>17.66879737657041</v>
+        <v>17.2438913143201</v>
       </c>
       <c r="O9" t="n">
-        <v>24.83690595209174</v>
+        <v>21.50448201789163</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="n">
-        <v>8.871518673934105</v>
+        <v>12.78931290264147</v>
       </c>
       <c r="B10" t="n">
-        <v>24.33797950257726</v>
+        <v>27.95513288348207</v>
       </c>
       <c r="C10" t="n">
-        <v>16.1629929341664</v>
+        <v>5.542397677384428</v>
       </c>
       <c r="D10" t="n">
-        <v>23.73202199082382</v>
+        <v>10.04420863906235</v>
       </c>
       <c r="E10" t="n">
-        <v>19.17170223677183</v>
+        <v>17.77647911017322</v>
       </c>
       <c r="F10" t="n">
-        <v>28.04752520561568</v>
+        <v>9.602590844918373</v>
       </c>
       <c r="G10" t="n">
-        <v>19.65927212675994</v>
+        <v>13.35001869729106</v>
       </c>
       <c r="H10" t="n">
-        <v>2.451348934149341</v>
+        <v>1.722129677228411</v>
       </c>
       <c r="I10" t="n">
-        <v>2.7773709496792</v>
+        <v>11.03198188628979</v>
       </c>
       <c r="J10" t="n">
-        <v>11.63548895398073</v>
+        <v>16.76329562101495</v>
       </c>
       <c r="K10" t="n">
-        <v>14.25778194432186</v>
+        <v>24.01852074106805</v>
       </c>
       <c r="L10" t="n">
-        <v>5.577956386599646</v>
+        <v>22.39552612028641</v>
       </c>
       <c r="M10" t="n">
-        <v>1.867982060663671</v>
+        <v>10.51064409650425</v>
       </c>
       <c r="N10" t="n">
-        <v>28.14770422666124</v>
+        <v>14.34315099529383</v>
       </c>
       <c r="O10" t="n">
-        <v>12.83150656343364</v>
+        <v>8.901257387151126</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="n">
-        <v>17.55984472306331</v>
+        <v>13.14758647698259</v>
       </c>
       <c r="B11" t="n">
-        <v>15.07264759232322</v>
+        <v>20.48030952289237</v>
       </c>
       <c r="C11" t="n">
-        <v>28.50112738058266</v>
+        <v>6.078492349624941</v>
       </c>
       <c r="D11" t="n">
-        <v>7.698780288728041</v>
+        <v>15.66942298570057</v>
       </c>
       <c r="E11" t="n">
-        <v>29.27326423597649</v>
+        <v>5.861167315695384</v>
       </c>
       <c r="F11" t="n">
-        <v>22.67059933666865</v>
+        <v>22.92140451517371</v>
       </c>
       <c r="G11" t="n">
-        <v>25.66667175762732</v>
+        <v>24.77410383624736</v>
       </c>
       <c r="H11" t="n">
-        <v>2.971640167613392</v>
+        <v>22.93041402784607</v>
       </c>
       <c r="I11" t="n">
-        <v>23.78858442793625</v>
+        <v>23.86734851940706</v>
       </c>
       <c r="J11" t="n">
-        <v>17.28345008519804</v>
+        <v>8.419760211949587</v>
       </c>
       <c r="K11" t="n">
-        <v>18.25819187732363</v>
+        <v>27.91046424709499</v>
       </c>
       <c r="L11" t="n">
-        <v>2.243129405044724</v>
+        <v>14.28698928920588</v>
       </c>
       <c r="M11" t="n">
-        <v>4.807266925054734</v>
+        <v>27.60853096486451</v>
       </c>
       <c r="N11" t="n">
-        <v>12.28489004394434</v>
+        <v>21.05788838293685</v>
       </c>
       <c r="O11" t="n">
-        <v>3.013282607751542</v>
+        <v>29.9214720156209</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="n">
-        <v>13.27065935336048</v>
+        <v>12.87284893647637</v>
       </c>
       <c r="B12" t="n">
-        <v>23.09161704854624</v>
+        <v>7.321300924394389</v>
       </c>
       <c r="C12" t="n">
-        <v>15.47499585761519</v>
+        <v>20.37823911267997</v>
       </c>
       <c r="D12" t="n">
-        <v>11.07938282915257</v>
+        <v>7.931702599577209</v>
       </c>
       <c r="E12" t="n">
-        <v>16.23716771423633</v>
+        <v>15.07433981712331</v>
       </c>
       <c r="F12" t="n">
-        <v>9.495829390176224</v>
+        <v>22.51562092900768</v>
       </c>
       <c r="G12" t="n">
-        <v>11.08140560964173</v>
+        <v>19.68029726492231</v>
       </c>
       <c r="H12" t="n">
-        <v>18.18331223854753</v>
+        <v>2.380982017536825</v>
       </c>
       <c r="I12" t="n">
-        <v>12.76315833387094</v>
+        <v>5.723296727042653</v>
       </c>
       <c r="J12" t="n">
-        <v>29.76769672005572</v>
+        <v>28.91971976610722</v>
       </c>
       <c r="K12" t="n">
-        <v>22.58657248842154</v>
+        <v>7.795921389559149</v>
       </c>
       <c r="L12" t="n">
-        <v>16.53506975641861</v>
+        <v>21.368981248342</v>
       </c>
       <c r="M12" t="n">
-        <v>18.19745037367591</v>
+        <v>16.66751768394892</v>
       </c>
       <c r="N12" t="n">
-        <v>26.12573491983354</v>
+        <v>5.191305531889839</v>
       </c>
       <c r="O12" t="n">
-        <v>29.6858940842997</v>
+        <v>16.30986653827399</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="n">
-        <v>7.505551813363915</v>
+        <v>11.38409583899061</v>
       </c>
       <c r="B13" t="n">
-        <v>24.03270056364362</v>
+        <v>4.393729294287832</v>
       </c>
       <c r="C13" t="n">
-        <v>26.03277467480209</v>
+        <v>6.661436790191807</v>
       </c>
       <c r="D13" t="n">
-        <v>2.745068206531383</v>
+        <v>4.282348756470161</v>
       </c>
       <c r="E13" t="n">
-        <v>29.88864349624915</v>
+        <v>28.09506930151939</v>
       </c>
       <c r="F13" t="n">
-        <v>5.580380103159774</v>
+        <v>23.20557937634998</v>
       </c>
       <c r="G13" t="n">
-        <v>24.40769383616466</v>
+        <v>4.130157728067699</v>
       </c>
       <c r="H13" t="n">
-        <v>23.49604110617765</v>
+        <v>2.586842153440894</v>
       </c>
       <c r="I13" t="n">
-        <v>10.13145211938455</v>
+        <v>15.23422438074079</v>
       </c>
       <c r="J13" t="n">
-        <v>29.49270672461223</v>
+        <v>26.06757407379948</v>
       </c>
       <c r="K13" t="n">
-        <v>28.95705246684448</v>
+        <v>15.81327078037232</v>
       </c>
       <c r="L13" t="n">
-        <v>1.088715970035635</v>
+        <v>27.77464927717223</v>
       </c>
       <c r="M13" t="n">
-        <v>13.90815096326752</v>
+        <v>25.78421838537085</v>
       </c>
       <c r="N13" t="n">
-        <v>21.35359587975941</v>
+        <v>4.011239984298193</v>
       </c>
       <c r="O13" t="n">
-        <v>2.007063872923983</v>
+        <v>20.28724031974253</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="n">
-        <v>7.010023844654921</v>
+        <v>6.820272518211079</v>
       </c>
       <c r="B14" t="n">
-        <v>2.359666224438888</v>
+        <v>26.15736283146289</v>
       </c>
       <c r="C14" t="n">
-        <v>24.3092901433392</v>
+        <v>14.44350209485315</v>
       </c>
       <c r="D14" t="n">
-        <v>7.333831331570906</v>
+        <v>20.23658713028516</v>
       </c>
       <c r="E14" t="n">
-        <v>17.45781580798906</v>
+        <v>21.90976619391834</v>
       </c>
       <c r="F14" t="n">
-        <v>23.83524389174948</v>
+        <v>20.72848403701386</v>
       </c>
       <c r="G14" t="n">
-        <v>12.39898897464736</v>
+        <v>17.3394669612568</v>
       </c>
       <c r="H14" t="n">
-        <v>27.84351217430019</v>
+        <v>28.3753912516888</v>
       </c>
       <c r="I14" t="n">
-        <v>29.36990158365435</v>
+        <v>27.47846726079839</v>
       </c>
       <c r="J14" t="n">
-        <v>1.543752671851612</v>
+        <v>21.72876512411175</v>
       </c>
       <c r="K14" t="n">
-        <v>28.7462423066763</v>
+        <v>16.6092475771182</v>
       </c>
       <c r="L14" t="n">
-        <v>7.856491806575601</v>
+        <v>5.505391559928768</v>
       </c>
       <c r="M14" t="n">
-        <v>16.23116416878525</v>
+        <v>4.306570994143156</v>
       </c>
       <c r="N14" t="n">
-        <v>13.96366207077308</v>
+        <v>24.67444124306629</v>
       </c>
       <c r="O14" t="n">
-        <v>14.81729513755321</v>
+        <v>19.18843641230858</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="n">
-        <v>25.94009981064387</v>
+        <v>10.61491848661818</v>
       </c>
       <c r="B15" t="n">
-        <v>22.82488883378111</v>
+        <v>1.301329795507729</v>
       </c>
       <c r="C15" t="n">
-        <v>8.954292276324885</v>
+        <v>23.17470076406565</v>
       </c>
       <c r="D15" t="n">
-        <v>18.9410811962099</v>
+        <v>1.865508259636456</v>
       </c>
       <c r="E15" t="n">
-        <v>3.087642686877868</v>
+        <v>25.28078642068363</v>
       </c>
       <c r="F15" t="n">
-        <v>28.13150848655003</v>
+        <v>8.300469936984037</v>
       </c>
       <c r="G15" t="n">
-        <v>9.005489079581631</v>
+        <v>23.97458171890923</v>
       </c>
       <c r="H15" t="n">
-        <v>14.0292291586839</v>
+        <v>8.878301832807477</v>
       </c>
       <c r="I15" t="n">
-        <v>16.22819478761007</v>
+        <v>12.88898550789792</v>
       </c>
       <c r="J15" t="n">
-        <v>23.71140900661353</v>
+        <v>29.21181414349279</v>
       </c>
       <c r="K15" t="n">
-        <v>26.18892310626952</v>
+        <v>21.08774988688578</v>
       </c>
       <c r="L15" t="n">
-        <v>5.340333986059015</v>
+        <v>15.5330257791087</v>
       </c>
       <c r="M15" t="n">
-        <v>7.118966232412073</v>
+        <v>14.43782707359506</v>
       </c>
       <c r="N15" t="n">
-        <v>1.498576338485525</v>
+        <v>17.54777872928039</v>
       </c>
       <c r="O15" t="n">
-        <v>22.48156783660458</v>
+        <v>16.72090132682687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>